<commit_message>
add file 12 from19990930to20150929 as train-data
</commit_message>
<xml_diff>
--- a/ROI/ROI.xlsx
+++ b/ROI/ROI.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="file9" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="file10" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="file10_anti" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="256">
   <si>
     <t xml:space="preserve">date</t>
   </si>
@@ -926,11 +927,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1019,7 +1020,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.4587628865979"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.319587628866"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3647,15 +3648,15 @@
   </sheetPr>
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J86" activeCellId="0" sqref="J86"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.639175257732"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.639175257732"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.639175257732"/>
+    <col collapsed="false" hidden="false" max="5" min="1" style="0" width="11.4587628865979"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="4" width="11.4587628865979"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.4587628865979"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3700,7 +3701,7 @@
       <c r="D2" s="0" t="n">
         <v>17888.35</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="6" t="n">
         <f aca="false">B2-D2</f>
         <v>-659.879999999997</v>
       </c>
@@ -3726,7 +3727,7 @@
       <c r="D3" s="0" t="n">
         <v>17729.68</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="6" t="n">
         <f aca="false">B3-D3</f>
         <v>-503.75</v>
       </c>
@@ -3752,7 +3753,7 @@
       <c r="D4" s="0" t="n">
         <v>17477.67</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="6" t="n">
         <f aca="false">B4-D4</f>
         <v>-296.789999999997</v>
       </c>
@@ -3778,7 +3779,7 @@
       <c r="D5" s="0" t="n">
         <v>17847.63</v>
       </c>
-      <c r="E5" s="0" t="n">
+      <c r="E5" s="6" t="n">
         <f aca="false">B5-D5</f>
         <v>-322.52</v>
       </c>
@@ -3804,7 +3805,7 @@
       <c r="D6" s="0" t="n">
         <v>17730.51</v>
       </c>
-      <c r="E6" s="0" t="n">
+      <c r="E6" s="6" t="n">
         <f aca="false">B6-D6</f>
         <v>-80.9399999999987</v>
       </c>
@@ -3830,7 +3831,7 @@
       <c r="D7" s="0" t="n">
         <v>17568</v>
       </c>
-      <c r="E7" s="0" t="n">
+      <c r="E7" s="6" t="n">
         <f aca="false">B7-D7</f>
         <v>40.8899999999994</v>
       </c>
@@ -3856,7 +3857,7 @@
       <c r="D8" s="0" t="n">
         <v>17492.3</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="E8" s="6" t="n">
         <f aca="false">B8-D8</f>
         <v>94.3899999999994</v>
       </c>
@@ -3882,7 +3883,7 @@
       <c r="D9" s="0" t="n">
         <v>17574.75</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="E9" s="6" t="n">
         <f aca="false">B9-D9</f>
         <v>196.75</v>
       </c>
@@ -3908,7 +3909,7 @@
       <c r="D10" s="0" t="n">
         <v>17265.21</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="E10" s="6" t="n">
         <f aca="false">B10-D10</f>
         <v>491.389999999999</v>
       </c>
@@ -3934,7 +3935,7 @@
       <c r="D11" s="0" t="n">
         <v>17368.5</v>
       </c>
-      <c r="E11" s="0" t="n">
+      <c r="E11" s="6" t="n">
         <f aca="false">B11-D11</f>
         <v>304.119999999999</v>
       </c>
@@ -3960,7 +3961,7 @@
       <c r="D12" s="0" t="n">
         <v>17524.91</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="E12" s="6" t="n">
         <f aca="false">B12-D12</f>
         <v>294.830000000002</v>
       </c>
@@ -3986,7 +3987,7 @@
       <c r="D13" s="0" t="n">
         <v>17749.09</v>
       </c>
-      <c r="E13" s="0" t="n">
+      <c r="E13" s="6" t="n">
         <f aca="false">B13-D13</f>
         <v>180.490000000002</v>
       </c>
@@ -4012,7 +4013,7 @@
       <c r="D14" s="0" t="n">
         <v>17495.84</v>
       </c>
-      <c r="E14" s="0" t="n">
+      <c r="E14" s="6" t="n">
         <f aca="false">B14-D14</f>
         <v>375.41</v>
       </c>
@@ -4038,7 +4039,7 @@
       <c r="D15" s="0" t="n">
         <v>17128.55</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="E15" s="6" t="n">
         <f aca="false">B15-D15</f>
         <v>726.670000000002</v>
       </c>
@@ -4064,7 +4065,7 @@
       <c r="D16" s="0" t="n">
         <v>17251.62</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="E16" s="6" t="n">
         <f aca="false">B16-D16</f>
         <v>649.16</v>
       </c>
@@ -4090,7 +4091,7 @@
       <c r="D17" s="0" t="n">
         <v>17417.27</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="E17" s="6" t="n">
         <f aca="false">B17-D17</f>
         <v>306.860000000001</v>
       </c>
@@ -4116,7 +4117,7 @@
       <c r="D18" s="0" t="n">
         <v>17602.61</v>
       </c>
-      <c r="E18" s="0" t="n">
+      <c r="E18" s="6" t="n">
         <f aca="false">B18-D18</f>
         <v>166.889999999999</v>
       </c>
@@ -4142,7 +4143,7 @@
       <c r="D19" s="0" t="n">
         <v>17552.17</v>
       </c>
-      <c r="E19" s="0" t="n">
+      <c r="E19" s="6" t="n">
         <f aca="false">B19-D19</f>
         <v>139.760000000002</v>
       </c>
@@ -4168,7 +4169,7 @@
       <c r="D20" s="0" t="n">
         <v>17528.27</v>
       </c>
-      <c r="E20" s="0" t="n">
+      <c r="E20" s="6" t="n">
         <f aca="false">B20-D20</f>
         <v>-89.0200000000004</v>
       </c>
@@ -4324,7 +4325,7 @@
       <c r="D26" s="0" t="n">
         <v>16906.51</v>
       </c>
-      <c r="E26" s="0" t="n">
+      <c r="E26" s="6" t="n">
         <f aca="false">B26-D26</f>
         <v>917.100000000002</v>
       </c>
@@ -4350,7 +4351,7 @@
       <c r="D27" s="0" t="n">
         <v>16514.1</v>
       </c>
-      <c r="E27" s="0" t="n">
+      <c r="E27" s="6" t="n">
         <f aca="false">B27-D27</f>
         <v>1256.8</v>
       </c>
@@ -4376,7 +4377,7 @@
       <c r="D28" s="0" t="n">
         <v>16346.45</v>
       </c>
-      <c r="E28" s="0" t="n">
+      <c r="E28" s="6" t="n">
         <f aca="false">B28-D28</f>
         <v>1474.36</v>
       </c>
@@ -4402,7 +4403,7 @@
       <c r="D29" s="0" t="n">
         <v>16398.57</v>
       </c>
-      <c r="E29" s="0" t="n">
+      <c r="E29" s="6" t="n">
         <f aca="false">B29-D29</f>
         <v>1407.47</v>
       </c>
@@ -4428,7 +4429,7 @@
       <c r="D30" s="0" t="n">
         <v>16516.22</v>
       </c>
-      <c r="E30" s="0" t="n">
+      <c r="E30" s="6" t="n">
         <f aca="false">B30-D30</f>
         <v>1286.62</v>
       </c>
@@ -4454,7 +4455,7 @@
       <c r="D31" s="0" t="n">
         <v>16151.41</v>
       </c>
-      <c r="E31" s="0" t="n">
+      <c r="E31" s="6" t="n">
         <f aca="false">B31-D31</f>
         <v>1568.31</v>
       </c>
@@ -4480,7 +4481,7 @@
       <c r="D32" s="0" t="n">
         <v>16379.05</v>
       </c>
-      <c r="E32" s="0" t="n">
+      <c r="E32" s="6" t="n">
         <f aca="false">B32-D32</f>
         <v>1504.09</v>
       </c>
@@ -4506,7 +4507,7 @@
       <c r="D33" s="0" t="n">
         <v>15988.08</v>
       </c>
-      <c r="E33" s="0" t="n">
+      <c r="E33" s="6" t="n">
         <f aca="false">B33-D33</f>
         <v>1753.49</v>
       </c>
@@ -4558,7 +4559,7 @@
       <c r="D35" s="0" t="n">
         <v>15766.74</v>
       </c>
-      <c r="E35" s="0" t="n">
+      <c r="E35" s="6" t="n">
         <f aca="false">B35-D35</f>
         <v>2078.75</v>
       </c>
@@ -4584,7 +4585,7 @@
       <c r="D36" s="0" t="n">
         <v>15882.68</v>
       </c>
-      <c r="E36" s="6" t="n">
+      <c r="E36" s="7" t="n">
         <f aca="false">D36-B36</f>
         <v>-1821.31</v>
       </c>
@@ -4610,7 +4611,7 @@
       <c r="D37" s="0" t="n">
         <v>16093.51</v>
       </c>
-      <c r="E37" s="6" t="n">
+      <c r="E37" s="7" t="n">
         <f aca="false">D37-B37</f>
         <v>-1464.67</v>
       </c>
@@ -4636,7 +4637,7 @@
       <c r="D38" s="0" t="n">
         <v>15885.22</v>
       </c>
-      <c r="E38" s="6" t="n">
+      <c r="E38" s="7" t="n">
         <f aca="false">D38-B38</f>
         <v>-1607.95</v>
       </c>
@@ -4662,7 +4663,7 @@
       <c r="D39" s="0" t="n">
         <v>16167.23</v>
       </c>
-      <c r="E39" s="6" t="n">
+      <c r="E39" s="7" t="n">
         <f aca="false">D39-B39</f>
         <v>-1407.52</v>
       </c>
@@ -4688,7 +4689,7 @@
       <c r="D40" s="0" t="n">
         <v>15944.46</v>
       </c>
-      <c r="E40" s="6" t="n">
+      <c r="E40" s="7" t="n">
         <f aca="false">D40-B40</f>
         <v>-1332.65</v>
       </c>
@@ -4714,7 +4715,7 @@
       <c r="D41" s="0" t="n">
         <v>16069.64</v>
       </c>
-      <c r="E41" s="6" t="n">
+      <c r="E41" s="7" t="n">
         <f aca="false">D41-B41</f>
         <v>-1305.14</v>
       </c>
@@ -4740,7 +4741,7 @@
       <c r="D42" s="0" t="n">
         <v>16466.3</v>
       </c>
-      <c r="E42" s="6" t="n">
+      <c r="E42" s="7" t="n">
         <f aca="false">D42-B42</f>
         <v>-1064.55</v>
       </c>
@@ -4766,7 +4767,7 @@
       <c r="D43" s="0" t="n">
         <v>16449.18</v>
       </c>
-      <c r="E43" s="6" t="n">
+      <c r="E43" s="7" t="n">
         <f aca="false">D43-B43</f>
         <v>-1307.36</v>
       </c>
@@ -4792,7 +4793,7 @@
       <c r="D44" s="0" t="n">
         <v>16153.54</v>
       </c>
-      <c r="E44" s="6" t="n">
+      <c r="E44" s="7" t="n">
         <f aca="false">D44-B44</f>
         <v>-1341.5</v>
       </c>
@@ -4818,7 +4819,7 @@
       <c r="D45" s="0" t="n">
         <v>16336.66</v>
       </c>
-      <c r="E45" s="6" t="n">
+      <c r="E45" s="7" t="n">
         <f aca="false">D45-B45</f>
         <v>-818.279999999999</v>
       </c>
@@ -4844,7 +4845,7 @@
       <c r="D46" s="0" t="n">
         <v>16416.58</v>
       </c>
-      <c r="E46" s="6" t="n">
+      <c r="E46" s="7" t="n">
         <f aca="false">D46-B46</f>
         <v>-836.969999999998</v>
       </c>
@@ -4870,7 +4871,7 @@
       <c r="D47" s="0" t="n">
         <v>16204.97</v>
       </c>
-      <c r="E47" s="6" t="n">
+      <c r="E47" s="7" t="n">
         <f aca="false">D47-B47</f>
         <v>-1222.66</v>
       </c>
@@ -4896,7 +4897,7 @@
       <c r="D48" s="0" t="n">
         <v>16027.05</v>
       </c>
-      <c r="E48" s="6" t="n">
+      <c r="E48" s="7" t="n">
         <f aca="false">D48-B48</f>
         <v>-1566.21</v>
       </c>
@@ -4922,7 +4923,7 @@
       <c r="D49" s="0" t="n">
         <v>16014.38</v>
       </c>
-      <c r="E49" s="6" t="n">
+      <c r="E49" s="7" t="n">
         <f aca="false">D49-B49</f>
         <v>-1521.28</v>
       </c>
@@ -4948,7 +4949,7 @@
       <c r="D50" s="0" t="n">
         <v>15914.74</v>
       </c>
-      <c r="E50" s="6" t="n">
+      <c r="E50" s="7" t="n">
         <f aca="false">D50-B50</f>
         <v>-1632.63</v>
       </c>
@@ -4974,7 +4975,7 @@
       <c r="D51" s="0" t="n">
         <v>15660.18</v>
       </c>
-      <c r="E51" s="7" t="n">
+      <c r="E51" s="6" t="n">
         <f aca="false">B51-D51</f>
         <v>2051.76</v>
       </c>
@@ -5000,7 +5001,7 @@
       <c r="D52" s="0" t="n">
         <v>15973.84</v>
       </c>
-      <c r="E52" s="7" t="n">
+      <c r="E52" s="6" t="n">
         <f aca="false">B52-D52</f>
         <v>1616.82</v>
       </c>
@@ -5026,7 +5027,7 @@
       <c r="D53" s="0" t="n">
         <v>16196.41</v>
       </c>
-      <c r="E53" s="7" t="n">
+      <c r="E53" s="6" t="n">
         <f aca="false">B53-D53</f>
         <v>1209.07</v>
       </c>
@@ -5988,7 +5989,7 @@
       <c r="D90" s="0" t="n">
         <v>17576.96</v>
       </c>
-      <c r="E90" s="7" t="n">
+      <c r="E90" s="6" t="n">
         <f aca="false">B90-D90</f>
         <v>-864.259999999998</v>
       </c>
@@ -6014,7 +6015,7 @@
       <c r="D91" s="0" t="n">
         <v>17556.41</v>
       </c>
-      <c r="E91" s="7" t="n">
+      <c r="E91" s="6" t="n">
         <f aca="false">B91-D91</f>
         <v>-922.259999999998</v>
       </c>
@@ -6040,7 +6041,7 @@
       <c r="D92" s="0" t="n">
         <v>17721.25</v>
       </c>
-      <c r="E92" s="7" t="n">
+      <c r="E92" s="6" t="n">
         <f aca="false">B92-D92</f>
         <v>-1175.58</v>
       </c>
@@ -6051,6 +6052,2430 @@
       <c r="G92" s="4" t="n">
         <f aca="false">SUM($F$2:F92)</f>
         <v>1.64297808032408</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,標準"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,標準"&amp;12頁 &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I92"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A68" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I90" activeCellId="0" sqref="I90"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="4" min="1" style="0" width="11.639175257732"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.4587628865979"/>
+    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="11.639175257732"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>17228.47</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>17888.35</v>
+      </c>
+      <c r="E2" s="6" t="n">
+        <f aca="false">D2-B2</f>
+        <v>659.879999999997</v>
+      </c>
+      <c r="F2" s="4" t="n">
+        <f aca="false">E2/B2</f>
+        <v>0.0383017180283564</v>
+      </c>
+      <c r="G2" s="4" t="n">
+        <f aca="false">SUM($F$2:F2)</f>
+        <v>0.0383017180283564</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>17225.93</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>17729.68</v>
+      </c>
+      <c r="E3" s="6" t="n">
+        <f aca="false">D3-B3</f>
+        <v>503.75</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <f aca="false">E3/B3</f>
+        <v>0.0292437041135079</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <f aca="false">SUM($F$2:F3)</f>
+        <v>0.0675454221418643</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="5" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>17180.88</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>17477.67</v>
+      </c>
+      <c r="E4" s="6" t="n">
+        <f aca="false">D4-B4</f>
+        <v>296.789999999997</v>
+      </c>
+      <c r="F4" s="4" t="n">
+        <f aca="false">E4/B4</f>
+        <v>0.0172744353024989</v>
+      </c>
+      <c r="G4" s="4" t="n">
+        <f aca="false">SUM($F$2:F4)</f>
+        <v>0.0848198574443632</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>17525.11</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>17847.63</v>
+      </c>
+      <c r="E5" s="6" t="n">
+        <f aca="false">D5-B5</f>
+        <v>322.52</v>
+      </c>
+      <c r="F5" s="4" t="n">
+        <f aca="false">E5/B5</f>
+        <v>0.0184033081675379</v>
+      </c>
+      <c r="G5" s="4" t="n">
+        <f aca="false">SUM($F$2:F5)</f>
+        <v>0.103223165611901</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="5" t="s">
+        <v>144</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>17649.57</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>17730.51</v>
+      </c>
+      <c r="E6" s="6" t="n">
+        <f aca="false">D6-B6</f>
+        <v>80.9399999999987</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <f aca="false">E6/B6</f>
+        <v>0.00458594741968211</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <f aca="false">SUM($F$2:F6)</f>
+        <v>0.107809113031583</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>17608.89</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>17568</v>
+      </c>
+      <c r="E7" s="6" t="n">
+        <f aca="false">D7-B7</f>
+        <v>-40.8899999999994</v>
+      </c>
+      <c r="F7" s="4" t="n">
+        <f aca="false">E7/B7</f>
+        <v>-0.00232212251879587</v>
+      </c>
+      <c r="G7" s="4" t="n">
+        <f aca="false">SUM($F$2:F7)</f>
+        <v>0.105486990512787</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>17586.69</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>17492.3</v>
+      </c>
+      <c r="E8" s="6" t="n">
+        <f aca="false">D8-B8</f>
+        <v>-94.3899999999994</v>
+      </c>
+      <c r="F8" s="4" t="n">
+        <f aca="false">E8/B8</f>
+        <v>-0.0053671270716661</v>
+      </c>
+      <c r="G8" s="4" t="n">
+        <f aca="false">SUM($F$2:F8)</f>
+        <v>0.100119863441121</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>17771.5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>17574.75</v>
+      </c>
+      <c r="E9" s="6" t="n">
+        <f aca="false">D9-B9</f>
+        <v>-196.75</v>
+      </c>
+      <c r="F9" s="4" t="n">
+        <f aca="false">E9/B9</f>
+        <v>-0.0110710969811215</v>
+      </c>
+      <c r="G9" s="4" t="n">
+        <f aca="false">SUM($F$2:F9)</f>
+        <v>0.0890487664599998</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>17756.6</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>17265.21</v>
+      </c>
+      <c r="E10" s="6" t="n">
+        <f aca="false">D10-B10</f>
+        <v>-491.389999999999</v>
+      </c>
+      <c r="F10" s="4" t="n">
+        <f aca="false">E10/B10</f>
+        <v>-0.0276736537400178</v>
+      </c>
+      <c r="G10" s="4" t="n">
+        <f aca="false">SUM($F$2:F10)</f>
+        <v>0.0613751127199821</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="5" t="s">
+        <v>154</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>17672.62</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>17368.5</v>
+      </c>
+      <c r="E11" s="6" t="n">
+        <f aca="false">D11-B11</f>
+        <v>-304.119999999999</v>
+      </c>
+      <c r="F11" s="4" t="n">
+        <f aca="false">E11/B11</f>
+        <v>-0.0172085406691254</v>
+      </c>
+      <c r="G11" s="4" t="n">
+        <f aca="false">SUM($F$2:F11)</f>
+        <v>0.0441665720508567</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>17819.74</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>17524.91</v>
+      </c>
+      <c r="E12" s="6" t="n">
+        <f aca="false">D12-B12</f>
+        <v>-294.830000000002</v>
+      </c>
+      <c r="F12" s="4" t="n">
+        <f aca="false">E12/B12</f>
+        <v>-0.0165451347774997</v>
+      </c>
+      <c r="G12" s="4" t="n">
+        <f aca="false">SUM($F$2:F12)</f>
+        <v>0.027621437273357</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="5" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>17929.58</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>17749.09</v>
+      </c>
+      <c r="E13" s="6" t="n">
+        <f aca="false">D13-B13</f>
+        <v>-180.490000000002</v>
+      </c>
+      <c r="F13" s="4" t="n">
+        <f aca="false">E13/B13</f>
+        <v>-0.0100666050180764</v>
+      </c>
+      <c r="G13" s="4" t="n">
+        <f aca="false">SUM($F$2:F13)</f>
+        <v>0.0175548322552806</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>17871.25</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>17495.84</v>
+      </c>
+      <c r="E14" s="6" t="n">
+        <f aca="false">D14-B14</f>
+        <v>-375.41</v>
+      </c>
+      <c r="F14" s="4" t="n">
+        <f aca="false">E14/B14</f>
+        <v>-0.0210063649716724</v>
+      </c>
+      <c r="G14" s="4" t="n">
+        <f aca="false">SUM($F$2:F14)</f>
+        <v>-0.00345153271639173</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="s">
+        <v>162</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>17855.22</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>17128.55</v>
+      </c>
+      <c r="E15" s="6" t="n">
+        <f aca="false">D15-B15</f>
+        <v>-726.670000000002</v>
+      </c>
+      <c r="F15" s="4" t="n">
+        <f aca="false">E15/B15</f>
+        <v>-0.0406979023501252</v>
+      </c>
+      <c r="G15" s="4" t="n">
+        <f aca="false">SUM($F$2:F15)</f>
+        <v>-0.0441494350665169</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="5" t="s">
+        <v>164</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>17900.78</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>17251.62</v>
+      </c>
+      <c r="E16" s="6" t="n">
+        <f aca="false">D16-B16</f>
+        <v>-649.16</v>
+      </c>
+      <c r="F16" s="4" t="n">
+        <f aca="false">E16/B16</f>
+        <v>-0.0362643415538317</v>
+      </c>
+      <c r="G16" s="4" t="n">
+        <f aca="false">SUM($F$2:F16)</f>
+        <v>-0.0804137766203486</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="5" t="s">
+        <v>166</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>17724.13</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>17417.27</v>
+      </c>
+      <c r="E17" s="6" t="n">
+        <f aca="false">D17-B17</f>
+        <v>-306.860000000001</v>
+      </c>
+      <c r="F17" s="4" t="n">
+        <f aca="false">E17/B17</f>
+        <v>-0.0173131205875832</v>
+      </c>
+      <c r="G17" s="4" t="n">
+        <f aca="false">SUM($F$2:F17)</f>
+        <v>-0.0977268972079318</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>17769.5</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>17602.61</v>
+      </c>
+      <c r="E18" s="6" t="n">
+        <f aca="false">D18-B18</f>
+        <v>-166.889999999999</v>
+      </c>
+      <c r="F18" s="4" t="n">
+        <f aca="false">E18/B18</f>
+        <v>-0.00939193562002304</v>
+      </c>
+      <c r="G18" s="4" t="n">
+        <f aca="false">SUM($F$2:F18)</f>
+        <v>-0.107118832827955</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>17691.93</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>17552.17</v>
+      </c>
+      <c r="E19" s="6" t="n">
+        <f aca="false">D19-B19</f>
+        <v>-139.760000000002</v>
+      </c>
+      <c r="F19" s="4" t="n">
+        <f aca="false">E19/B19</f>
+        <v>-0.00789964690115787</v>
+      </c>
+      <c r="G19" s="4" t="n">
+        <f aca="false">SUM($F$2:F19)</f>
+        <v>-0.115018479729113</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>17439.25</v>
+      </c>
+      <c r="C20" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>17528.27</v>
+      </c>
+      <c r="E20" s="6" t="n">
+        <f aca="false">D20-B20</f>
+        <v>89.0200000000004</v>
+      </c>
+      <c r="F20" s="4" t="n">
+        <f aca="false">E20/B20</f>
+        <v>0.00510457731840535</v>
+      </c>
+      <c r="G20" s="4" t="n">
+        <f aca="false">SUM($F$2:F20)</f>
+        <v>-0.109913902410707</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>17229.94</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>17720.98</v>
+      </c>
+      <c r="E21" s="0" t="n">
+        <f aca="false">B21-D21</f>
+        <v>-491.040000000001</v>
+      </c>
+      <c r="F21" s="4" t="n">
+        <f aca="false">E21/B21</f>
+        <v>-0.0284992286682369</v>
+      </c>
+      <c r="G21" s="4" t="n">
+        <f aca="false">SUM($F$2:F21)</f>
+        <v>-0.138413131078944</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>17486.99</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>17603.87</v>
+      </c>
+      <c r="E22" s="0" t="n">
+        <f aca="false">B22-D22</f>
+        <v>-116.879999999997</v>
+      </c>
+      <c r="F22" s="4" t="n">
+        <f aca="false">E22/B22</f>
+        <v>-0.00668382609013886</v>
+      </c>
+      <c r="G22" s="4" t="n">
+        <f aca="false">SUM($F$2:F22)</f>
+        <v>-0.145096957169083</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>17485.49</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>17425.03</v>
+      </c>
+      <c r="E23" s="0" t="n">
+        <f aca="false">B23-D23</f>
+        <v>60.4600000000028</v>
+      </c>
+      <c r="F23" s="4" t="n">
+        <f aca="false">E23/B23</f>
+        <v>0.00345772409008857</v>
+      </c>
+      <c r="G23" s="4" t="n">
+        <f aca="false">SUM($F$2:F23)</f>
+        <v>-0.141639233078995</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="5" t="s">
+        <v>180</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>17739.83</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>17148.94</v>
+      </c>
+      <c r="E24" s="0" t="n">
+        <f aca="false">B24-D24</f>
+        <v>590.890000000003</v>
+      </c>
+      <c r="F24" s="4" t="n">
+        <f aca="false">E24/B24</f>
+        <v>0.0333086619206612</v>
+      </c>
+      <c r="G24" s="4" t="n">
+        <f aca="false">SUM($F$2:F24)</f>
+        <v>-0.108330571158333</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>17732.75</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>17158.66</v>
+      </c>
+      <c r="E25" s="0" t="n">
+        <f aca="false">B25-D25</f>
+        <v>574.09</v>
+      </c>
+      <c r="F25" s="4" t="n">
+        <f aca="false">E25/B25</f>
+        <v>0.0323745611932723</v>
+      </c>
+      <c r="G25" s="4" t="n">
+        <f aca="false">SUM($F$2:F25)</f>
+        <v>-0.075956009965061</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>17823.61</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>16906.51</v>
+      </c>
+      <c r="E26" s="6" t="n">
+        <f aca="false">D26-B26</f>
+        <v>-917.100000000002</v>
+      </c>
+      <c r="F26" s="4" t="n">
+        <f aca="false">E26/B26</f>
+        <v>-0.0514542227977386</v>
+      </c>
+      <c r="G26" s="4" t="n">
+        <f aca="false">SUM($F$2:F26)</f>
+        <v>-0.1274102327628</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>17770.9</v>
+      </c>
+      <c r="C27" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>16514.1</v>
+      </c>
+      <c r="E27" s="6" t="n">
+        <f aca="false">D27-B27</f>
+        <v>-1256.8</v>
+      </c>
+      <c r="F27" s="4" t="n">
+        <f aca="false">E27/B27</f>
+        <v>-0.0707223607133011</v>
+      </c>
+      <c r="G27" s="4" t="n">
+        <f aca="false">SUM($F$2:F27)</f>
+        <v>-0.198132593476101</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>17820.81</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>16346.45</v>
+      </c>
+      <c r="E28" s="6" t="n">
+        <f aca="false">D28-B28</f>
+        <v>-1474.36</v>
+      </c>
+      <c r="F28" s="4" t="n">
+        <f aca="false">E28/B28</f>
+        <v>-0.0827324908351529</v>
+      </c>
+      <c r="G28" s="4" t="n">
+        <f aca="false">SUM($F$2:F28)</f>
+        <v>-0.280865084311254</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>17806.04</v>
+      </c>
+      <c r="C29" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>16398.57</v>
+      </c>
+      <c r="E29" s="6" t="n">
+        <f aca="false">D29-B29</f>
+        <v>-1407.47</v>
+      </c>
+      <c r="F29" s="4" t="n">
+        <f aca="false">E29/B29</f>
+        <v>-0.0790445264640538</v>
+      </c>
+      <c r="G29" s="4" t="n">
+        <f aca="false">SUM($F$2:F29)</f>
+        <v>-0.359909610775307</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>17802.84</v>
+      </c>
+      <c r="C30" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>16516.22</v>
+      </c>
+      <c r="E30" s="6" t="n">
+        <f aca="false">D30-B30</f>
+        <v>-1286.62</v>
+      </c>
+      <c r="F30" s="4" t="n">
+        <f aca="false">E30/B30</f>
+        <v>-0.072270491674362</v>
+      </c>
+      <c r="G30" s="4" t="n">
+        <f aca="false">SUM($F$2:F30)</f>
+        <v>-0.432180102449669</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>17719.72</v>
+      </c>
+      <c r="C31" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>16151.41</v>
+      </c>
+      <c r="E31" s="6" t="n">
+        <f aca="false">D31-B31</f>
+        <v>-1568.31</v>
+      </c>
+      <c r="F31" s="4" t="n">
+        <f aca="false">E31/B31</f>
+        <v>-0.0885064775289904</v>
+      </c>
+      <c r="G31" s="4" t="n">
+        <f aca="false">SUM($F$2:F31)</f>
+        <v>-0.52068657997866</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>17883.14</v>
+      </c>
+      <c r="C32" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>16379.05</v>
+      </c>
+      <c r="E32" s="6" t="n">
+        <f aca="false">D32-B32</f>
+        <v>-1504.09</v>
+      </c>
+      <c r="F32" s="4" t="n">
+        <f aca="false">E32/B32</f>
+        <v>-0.0841065942558186</v>
+      </c>
+      <c r="G32" s="4" t="n">
+        <f aca="false">SUM($F$2:F32)</f>
+        <v>-0.604793174234478</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>17741.57</v>
+      </c>
+      <c r="C33" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>15988.08</v>
+      </c>
+      <c r="E33" s="6" t="n">
+        <f aca="false">D33-B33</f>
+        <v>-1753.49</v>
+      </c>
+      <c r="F33" s="4" t="n">
+        <f aca="false">E33/B33</f>
+        <v>-0.0988351087305126</v>
+      </c>
+      <c r="G33" s="4" t="n">
+        <f aca="false">SUM($F$2:F33)</f>
+        <v>-0.703628282964991</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>17482.68</v>
+      </c>
+      <c r="C34" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>16016.02</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <f aca="false">B34-D34</f>
+        <v>1466.66</v>
+      </c>
+      <c r="F34" s="4" t="n">
+        <f aca="false">E34/B34</f>
+        <v>0.0838921721383678</v>
+      </c>
+      <c r="G34" s="4" t="n">
+        <f aca="false">SUM($F$2:F34)</f>
+        <v>-0.619736110826623</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>17845.49</v>
+      </c>
+      <c r="C35" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>15766.74</v>
+      </c>
+      <c r="E35" s="6" t="n">
+        <f aca="false">D35-B35</f>
+        <v>-2078.75</v>
+      </c>
+      <c r="F35" s="4" t="n">
+        <f aca="false">E35/B35</f>
+        <v>-0.11648601411337</v>
+      </c>
+      <c r="G35" s="4" t="n">
+        <f aca="false">SUM($F$2:F35)</f>
+        <v>-0.736222124939993</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="5" t="s">
+        <v>147</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>17703.99</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>15882.68</v>
+      </c>
+      <c r="E36" s="7" t="n">
+        <f aca="false">B36-D36</f>
+        <v>1821.31</v>
+      </c>
+      <c r="F36" s="4" t="n">
+        <f aca="false">E36/B36</f>
+        <v>0.102875679437234</v>
+      </c>
+      <c r="G36" s="4" t="n">
+        <f aca="false">SUM($F$2:F36)</f>
+        <v>-0.633346445502759</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>17558.18</v>
+      </c>
+      <c r="C37" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>16093.51</v>
+      </c>
+      <c r="E37" s="7" t="n">
+        <f aca="false">B37-D37</f>
+        <v>1464.67</v>
+      </c>
+      <c r="F37" s="4" t="n">
+        <f aca="false">E37/B37</f>
+        <v>0.083418099142394</v>
+      </c>
+      <c r="G37" s="4" t="n">
+        <f aca="false">SUM($F$2:F37)</f>
+        <v>-0.549928346360365</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="5" t="s">
+        <v>151</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>17493.17</v>
+      </c>
+      <c r="C38" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>15885.22</v>
+      </c>
+      <c r="E38" s="7" t="n">
+        <f aca="false">B38-D38</f>
+        <v>1607.95</v>
+      </c>
+      <c r="F38" s="4" t="n">
+        <f aca="false">E38/B38</f>
+        <v>0.091918731710719</v>
+      </c>
+      <c r="G38" s="4" t="n">
+        <f aca="false">SUM($F$2:F38)</f>
+        <v>-0.458009614649646</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="5" t="s">
+        <v>153</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>17574.75</v>
+      </c>
+      <c r="C39" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>16167.23</v>
+      </c>
+      <c r="E39" s="7" t="n">
+        <f aca="false">B39-D39</f>
+        <v>1407.52</v>
+      </c>
+      <c r="F39" s="4" t="n">
+        <f aca="false">E39/B39</f>
+        <v>0.0800876257130258</v>
+      </c>
+      <c r="G39" s="4" t="n">
+        <f aca="false">SUM($F$2:F39)</f>
+        <v>-0.37792198893662</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>17277.11</v>
+      </c>
+      <c r="C40" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>15944.46</v>
+      </c>
+      <c r="E40" s="7" t="n">
+        <f aca="false">B40-D40</f>
+        <v>1332.65</v>
+      </c>
+      <c r="F40" s="4" t="n">
+        <f aca="false">E40/B40</f>
+        <v>0.0771338493532773</v>
+      </c>
+      <c r="G40" s="4" t="n">
+        <f aca="false">SUM($F$2:F40)</f>
+        <v>-0.300788139583343</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>17374.78</v>
+      </c>
+      <c r="C41" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>16069.64</v>
+      </c>
+      <c r="E41" s="7" t="n">
+        <f aca="false">B41-D41</f>
+        <v>1305.14</v>
+      </c>
+      <c r="F41" s="4" t="n">
+        <f aca="false">E41/B41</f>
+        <v>0.0751169223437649</v>
+      </c>
+      <c r="G41" s="4" t="n">
+        <f aca="false">SUM($F$2:F41)</f>
+        <v>-0.225671217239578</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="5" t="s">
+        <v>159</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>17530.85</v>
+      </c>
+      <c r="C42" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D42" s="0" t="n">
+        <v>16466.3</v>
+      </c>
+      <c r="E42" s="7" t="n">
+        <f aca="false">B42-D42</f>
+        <v>1064.55</v>
+      </c>
+      <c r="F42" s="4" t="n">
+        <f aca="false">E42/B42</f>
+        <v>0.0607243801641107</v>
+      </c>
+      <c r="G42" s="4" t="n">
+        <f aca="false">SUM($F$2:F42)</f>
+        <v>-0.164946837075467</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>17756.54</v>
+      </c>
+      <c r="C43" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>16449.18</v>
+      </c>
+      <c r="E43" s="7" t="n">
+        <f aca="false">B43-D43</f>
+        <v>1307.36</v>
+      </c>
+      <c r="F43" s="4" t="n">
+        <f aca="false">E43/B43</f>
+        <v>0.0736269566030319</v>
+      </c>
+      <c r="G43" s="4" t="n">
+        <f aca="false">SUM($F$2:F43)</f>
+        <v>-0.0913198804724351</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>17495.04</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>16153.54</v>
+      </c>
+      <c r="E44" s="7" t="n">
+        <f aca="false">B44-D44</f>
+        <v>1341.5</v>
+      </c>
+      <c r="F44" s="4" t="n">
+        <f aca="false">E44/B44</f>
+        <v>0.0766788758413813</v>
+      </c>
+      <c r="G44" s="4" t="n">
+        <f aca="false">SUM($F$2:F44)</f>
+        <v>-0.0146410046310538</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>17154.94</v>
+      </c>
+      <c r="C45" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>16336.66</v>
+      </c>
+      <c r="E45" s="7" t="n">
+        <f aca="false">B45-D45</f>
+        <v>818.279999999999</v>
+      </c>
+      <c r="F45" s="4" t="n">
+        <f aca="false">E45/B45</f>
+        <v>0.0476993798870762</v>
+      </c>
+      <c r="G45" s="4" t="n">
+        <f aca="false">SUM($F$2:F45)</f>
+        <v>0.0330583752560224</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="5" t="s">
+        <v>167</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>17253.55</v>
+      </c>
+      <c r="C46" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>16416.58</v>
+      </c>
+      <c r="E46" s="7" t="n">
+        <f aca="false">B46-D46</f>
+        <v>836.969999999998</v>
+      </c>
+      <c r="F46" s="4" t="n">
+        <f aca="false">E46/B46</f>
+        <v>0.0485100167791555</v>
+      </c>
+      <c r="G46" s="4" t="n">
+        <f aca="false">SUM($F$2:F46)</f>
+        <v>0.0815683920351779</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>17427.63</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>16204.97</v>
+      </c>
+      <c r="E47" s="7" t="n">
+        <f aca="false">B47-D47</f>
+        <v>1222.66</v>
+      </c>
+      <c r="F47" s="4" t="n">
+        <f aca="false">E47/B47</f>
+        <v>0.0701564125472024</v>
+      </c>
+      <c r="G47" s="4" t="n">
+        <f aca="false">SUM($F$2:F47)</f>
+        <v>0.15172480458238</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>17593.26</v>
+      </c>
+      <c r="C48" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D48" s="0" t="n">
+        <v>16027.05</v>
+      </c>
+      <c r="E48" s="7" t="n">
+        <f aca="false">B48-D48</f>
+        <v>1566.21</v>
+      </c>
+      <c r="F48" s="4" t="n">
+        <f aca="false">E48/B48</f>
+        <v>0.0890232964214705</v>
+      </c>
+      <c r="G48" s="4" t="n">
+        <f aca="false">SUM($F$2:F48)</f>
+        <v>0.240748101003851</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B49" s="0" t="n">
+        <v>17535.66</v>
+      </c>
+      <c r="C49" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="D49" s="0" t="n">
+        <v>16014.38</v>
+      </c>
+      <c r="E49" s="7" t="n">
+        <f aca="false">B49-D49</f>
+        <v>1521.28</v>
+      </c>
+      <c r="F49" s="4" t="n">
+        <f aca="false">E49/B49</f>
+        <v>0.0867535068540335</v>
+      </c>
+      <c r="G49" s="4" t="n">
+        <f aca="false">SUM($F$2:F49)</f>
+        <v>0.327501607857884</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B50" s="0" t="n">
+        <v>17547.37</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="D50" s="0" t="n">
+        <v>15914.74</v>
+      </c>
+      <c r="E50" s="7" t="n">
+        <f aca="false">B50-D50</f>
+        <v>1632.63</v>
+      </c>
+      <c r="F50" s="4" t="n">
+        <f aca="false">E50/B50</f>
+        <v>0.09304129336761</v>
+      </c>
+      <c r="G50" s="4" t="n">
+        <f aca="false">SUM($F$2:F50)</f>
+        <v>0.420542901225494</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="B51" s="0" t="n">
+        <v>17711.94</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="D51" s="0" t="n">
+        <v>15660.18</v>
+      </c>
+      <c r="E51" s="6" t="n">
+        <f aca="false">D51-B51</f>
+        <v>-2051.76</v>
+      </c>
+      <c r="F51" s="4" t="n">
+        <f aca="false">E51/B51</f>
+        <v>-0.115840500814705</v>
+      </c>
+      <c r="G51" s="4" t="n">
+        <f aca="false">SUM($F$2:F51)</f>
+        <v>0.30470240041079</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="5" t="s">
+        <v>179</v>
+      </c>
+      <c r="B52" s="0" t="n">
+        <v>17590.66</v>
+      </c>
+      <c r="C52" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="D52" s="0" t="n">
+        <v>15973.84</v>
+      </c>
+      <c r="E52" s="6" t="n">
+        <f aca="false">D52-B52</f>
+        <v>-1616.82</v>
+      </c>
+      <c r="F52" s="4" t="n">
+        <f aca="false">E52/B52</f>
+        <v>-0.0919135495768777</v>
+      </c>
+      <c r="G52" s="4" t="n">
+        <f aca="false">SUM($F$2:F52)</f>
+        <v>0.212788850833912</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="5" t="s">
+        <v>181</v>
+      </c>
+      <c r="B53" s="0" t="n">
+        <v>17405.48</v>
+      </c>
+      <c r="C53" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="D53" s="0" t="n">
+        <v>16196.41</v>
+      </c>
+      <c r="E53" s="6" t="n">
+        <f aca="false">D53-B53</f>
+        <v>-1209.07</v>
+      </c>
+      <c r="F53" s="4" t="n">
+        <f aca="false">E53/B53</f>
+        <v>-0.0694649041566219</v>
+      </c>
+      <c r="G53" s="4" t="n">
+        <f aca="false">SUM($F$2:F53)</f>
+        <v>0.14332394667729</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="B54" s="0" t="n">
+        <v>17147.5</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="D54" s="0" t="n">
+        <v>16453.83</v>
+      </c>
+      <c r="E54" s="0" t="n">
+        <f aca="false">B54-D54</f>
+        <v>693.669999999998</v>
+      </c>
+      <c r="F54" s="4" t="n">
+        <f aca="false">E54/B54</f>
+        <v>0.0404531272780288</v>
+      </c>
+      <c r="G54" s="4" t="n">
+        <f aca="false">SUM($F$2:F54)</f>
+        <v>0.183777073955319</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="B55" s="0" t="n">
+        <v>17154.83</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="D55" s="0" t="n">
+        <v>16413.43</v>
+      </c>
+      <c r="E55" s="0" t="n">
+        <f aca="false">B55-D55</f>
+        <v>741.400000000002</v>
+      </c>
+      <c r="F55" s="4" t="n">
+        <f aca="false">E55/B55</f>
+        <v>0.043218149057729</v>
+      </c>
+      <c r="G55" s="4" t="n">
+        <f aca="false">SUM($F$2:F55)</f>
+        <v>0.226995223013048</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="B56" s="0" t="n">
+        <v>16888.36</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="D56" s="0" t="n">
+        <v>16391.99</v>
+      </c>
+      <c r="E56" s="0" t="n">
+        <f aca="false">B56-D56</f>
+        <v>496.369999999999</v>
+      </c>
+      <c r="F56" s="4" t="n">
+        <f aca="false">E56/B56</f>
+        <v>0.0293912493575456</v>
+      </c>
+      <c r="G56" s="4" t="n">
+        <f aca="false">SUM($F$2:F56)</f>
+        <v>0.256386472370593</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="B57" s="0" t="n">
+        <v>16519.17</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="D57" s="0" t="n">
+        <v>16620.66</v>
+      </c>
+      <c r="E57" s="0" t="n">
+        <f aca="false">B57-D57</f>
+        <v>-101.490000000002</v>
+      </c>
+      <c r="F57" s="4" t="n">
+        <f aca="false">E57/B57</f>
+        <v>-0.00614377114588697</v>
+      </c>
+      <c r="G57" s="4" t="n">
+        <f aca="false">SUM($F$2:F57)</f>
+        <v>0.250242701224706</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="B58" s="0" t="n">
+        <v>16358.71</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="D58" s="0" t="n">
+        <v>16431.78</v>
+      </c>
+      <c r="E58" s="0" t="n">
+        <f aca="false">B58-D58</f>
+        <v>-73.0699999999997</v>
+      </c>
+      <c r="F58" s="4" t="n">
+        <f aca="false">E58/B58</f>
+        <v>-0.00446673362386152</v>
+      </c>
+      <c r="G58" s="4" t="n">
+        <f aca="false">SUM($F$2:F58)</f>
+        <v>0.245775967600845</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="B59" s="0" t="n">
+        <v>16419.11</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="D59" s="0" t="n">
+        <v>16484.99</v>
+      </c>
+      <c r="E59" s="0" t="n">
+        <f aca="false">B59-D59</f>
+        <v>-65.880000000001</v>
+      </c>
+      <c r="F59" s="4" t="n">
+        <f aca="false">E59/B59</f>
+        <v>-0.00401239774872091</v>
+      </c>
+      <c r="G59" s="4" t="n">
+        <f aca="false">SUM($F$2:F59)</f>
+        <v>0.241763569852124</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="B60" s="0" t="n">
+        <v>16526.63</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="D60" s="0" t="n">
+        <v>16697.29</v>
+      </c>
+      <c r="E60" s="0" t="n">
+        <f aca="false">B60-D60</f>
+        <v>-170.66</v>
+      </c>
+      <c r="F60" s="4" t="n">
+        <f aca="false">E60/B60</f>
+        <v>-0.0103263641770887</v>
+      </c>
+      <c r="G60" s="4" t="n">
+        <f aca="false">SUM($F$2:F60)</f>
+        <v>0.231437205675035</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="B61" s="0" t="n">
+        <v>16159.01</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="D61" s="0" t="n">
+        <v>16639.97</v>
+      </c>
+      <c r="E61" s="0" t="n">
+        <f aca="false">B61-D61</f>
+        <v>-480.960000000001</v>
+      </c>
+      <c r="F61" s="4" t="n">
+        <f aca="false">E61/B61</f>
+        <v>-0.029764199663222</v>
+      </c>
+      <c r="G61" s="4" t="n">
+        <f aca="false">SUM($F$2:F61)</f>
+        <v>0.201673006011813</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="B62" s="0" t="n">
+        <v>16354.33</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="D62" s="0" t="n">
+        <v>16516.5</v>
+      </c>
+      <c r="E62" s="0" t="n">
+        <f aca="false">B62-D62</f>
+        <v>-162.17</v>
+      </c>
+      <c r="F62" s="4" t="n">
+        <f aca="false">E62/B62</f>
+        <v>-0.00991602835457032</v>
+      </c>
+      <c r="G62" s="4" t="n">
+        <f aca="false">SUM($F$2:F62)</f>
+        <v>0.191756977657243</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="B63" s="0" t="n">
+        <v>16009.45</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="D63" s="0" t="n">
+        <v>16865.08</v>
+      </c>
+      <c r="E63" s="0" t="n">
+        <f aca="false">B63-D63</f>
+        <v>-855.630000000001</v>
+      </c>
+      <c r="F63" s="4" t="n">
+        <f aca="false">E63/B63</f>
+        <v>-0.053445308864452</v>
+      </c>
+      <c r="G63" s="4" t="n">
+        <f aca="false">SUM($F$2:F63)</f>
+        <v>0.138311668792791</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="B64" s="0" t="n">
+        <v>15989.45</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>227</v>
+      </c>
+      <c r="D64" s="0" t="n">
+        <v>16899.32</v>
+      </c>
+      <c r="E64" s="0" t="n">
+        <f aca="false">B64-D64</f>
+        <v>-909.869999999999</v>
+      </c>
+      <c r="F64" s="4" t="n">
+        <f aca="false">E64/B64</f>
+        <v>-0.0569043963363342</v>
+      </c>
+      <c r="G64" s="4" t="n">
+        <f aca="false">SUM($F$2:F64)</f>
+        <v>0.0814072724564568</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="B65" s="0" t="n">
+        <v>15768.87</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="D65" s="0" t="n">
+        <v>16943.9</v>
+      </c>
+      <c r="E65" s="0" t="n">
+        <f aca="false">B65-D65</f>
+        <v>-1175.03</v>
+      </c>
+      <c r="F65" s="4" t="n">
+        <f aca="false">E65/B65</f>
+        <v>-0.0745158023371364</v>
+      </c>
+      <c r="G65" s="4" t="n">
+        <f aca="false">SUM($F$2:F65)</f>
+        <v>0.00689147011932038</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="B66" s="0" t="n">
+        <v>15921.1</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>229</v>
+      </c>
+      <c r="D66" s="0" t="n">
+        <v>17006.77</v>
+      </c>
+      <c r="E66" s="0" t="n">
+        <f aca="false">B66-D66</f>
+        <v>-1085.67</v>
+      </c>
+      <c r="F66" s="4" t="n">
+        <f aca="false">E66/B66</f>
+        <v>-0.0681906400939634</v>
+      </c>
+      <c r="G66" s="4" t="n">
+        <f aca="false">SUM($F$2:F66)</f>
+        <v>-0.061299169974643</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="B67" s="0" t="n">
+        <v>16086.46</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>230</v>
+      </c>
+      <c r="D67" s="0" t="n">
+        <v>17073.95</v>
+      </c>
+      <c r="E67" s="0" t="n">
+        <f aca="false">B67-D67</f>
+        <v>-987.490000000002</v>
+      </c>
+      <c r="F67" s="4" t="n">
+        <f aca="false">E67/B67</f>
+        <v>-0.0613864081967072</v>
+      </c>
+      <c r="G67" s="4" t="n">
+        <f aca="false">SUM($F$2:F67)</f>
+        <v>-0.12268557817135</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="B68" s="0" t="n">
+        <v>15893.16</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D68" s="0" t="n">
+        <v>16964.1</v>
+      </c>
+      <c r="E68" s="0" t="n">
+        <f aca="false">B68-D68</f>
+        <v>-1070.94</v>
+      </c>
+      <c r="F68" s="4" t="n">
+        <f aca="false">E68/B68</f>
+        <v>-0.0673837046880544</v>
+      </c>
+      <c r="G68" s="4" t="n">
+        <f aca="false">SUM($F$2:F68)</f>
+        <v>-0.190069282859405</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="B69" s="0" t="n">
+        <v>16168.74</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="D69" s="0" t="n">
+        <v>17000.36</v>
+      </c>
+      <c r="E69" s="0" t="n">
+        <f aca="false">B69-D69</f>
+        <v>-831.620000000001</v>
+      </c>
+      <c r="F69" s="4" t="n">
+        <f aca="false">E69/B69</f>
+        <v>-0.0514338161167785</v>
+      </c>
+      <c r="G69" s="4" t="n">
+        <f aca="false">SUM($F$2:F69)</f>
+        <v>-0.241503098976183</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="B70" s="0" t="n">
+        <v>15960.28</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="D70" s="0" t="n">
+        <v>16995.13</v>
+      </c>
+      <c r="E70" s="0" t="n">
+        <f aca="false">B70-D70</f>
+        <v>-1034.85</v>
+      </c>
+      <c r="F70" s="4" t="n">
+        <f aca="false">E70/B70</f>
+        <v>-0.0648390880360495</v>
+      </c>
+      <c r="G70" s="4" t="n">
+        <f aca="false">SUM($F$2:F70)</f>
+        <v>-0.306342187012233</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="B71" s="0" t="n">
+        <v>16090.26</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>234</v>
+      </c>
+      <c r="D71" s="0" t="n">
+        <v>17213.31</v>
+      </c>
+      <c r="E71" s="0" t="n">
+        <f aca="false">B71-D71</f>
+        <v>-1123.05</v>
+      </c>
+      <c r="F71" s="4" t="n">
+        <f aca="false">E71/B71</f>
+        <v>-0.069796883331904</v>
+      </c>
+      <c r="G71" s="4" t="n">
+        <f aca="false">SUM($F$2:F71)</f>
+        <v>-0.376139070344137</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="B72" s="0" t="n">
+        <v>16442.06</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="D72" s="0" t="n">
+        <v>17229.13</v>
+      </c>
+      <c r="E72" s="0" t="n">
+        <f aca="false">B72-D72</f>
+        <v>-787.07</v>
+      </c>
+      <c r="F72" s="4" t="n">
+        <f aca="false">E72/B72</f>
+        <v>-0.0478693059142224</v>
+      </c>
+      <c r="G72" s="4" t="n">
+        <f aca="false">SUM($F$2:F72)</f>
+        <v>-0.424008376258359</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="B73" s="0" t="n">
+        <v>16420.21</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="D73" s="0" t="n">
+        <v>17251.53</v>
+      </c>
+      <c r="E73" s="0" t="n">
+        <f aca="false">B73-D73</f>
+        <v>-831.32</v>
+      </c>
+      <c r="F73" s="4" t="n">
+        <f aca="false">E73/B73</f>
+        <v>-0.0506278543331662</v>
+      </c>
+      <c r="G73" s="4" t="n">
+        <f aca="false">SUM($F$2:F73)</f>
+        <v>-0.474636230591525</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="B74" s="0" t="n">
+        <v>16186.2</v>
+      </c>
+      <c r="C74" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="D74" s="0" t="n">
+        <v>17325.76</v>
+      </c>
+      <c r="E74" s="0" t="n">
+        <f aca="false">B74-D74</f>
+        <v>-1139.56</v>
+      </c>
+      <c r="F74" s="4" t="n">
+        <f aca="false">E74/B74</f>
+        <v>-0.0704031829583224</v>
+      </c>
+      <c r="G74" s="4" t="n">
+        <f aca="false">SUM($F$2:F74)</f>
+        <v>-0.545039413549848</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="B75" s="0" t="n">
+        <v>16329.67</v>
+      </c>
+      <c r="C75" s="5" t="s">
+        <v>238</v>
+      </c>
+      <c r="D75" s="0" t="n">
+        <v>17481.49</v>
+      </c>
+      <c r="E75" s="0" t="n">
+        <f aca="false">B75-D75</f>
+        <v>-1151.82</v>
+      </c>
+      <c r="F75" s="4" t="n">
+        <f aca="false">E75/B75</f>
+        <v>-0.0705354119219802</v>
+      </c>
+      <c r="G75" s="4" t="n">
+        <f aca="false">SUM($F$2:F75)</f>
+        <v>-0.615574825471828</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="B76" s="0" t="n">
+        <v>16417.95</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="D76" s="0" t="n">
+        <v>17602.3</v>
+      </c>
+      <c r="E76" s="0" t="n">
+        <f aca="false">B76-D76</f>
+        <v>-1184.35</v>
+      </c>
+      <c r="F76" s="4" t="n">
+        <f aca="false">E76/B76</f>
+        <v>-0.0721375080323669</v>
+      </c>
+      <c r="G76" s="4" t="n">
+        <f aca="false">SUM($F$2:F76)</f>
+        <v>-0.687712333504195</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="B77" s="0" t="n">
+        <v>16147.51</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="D77" s="0" t="n">
+        <v>17623.87</v>
+      </c>
+      <c r="E77" s="0" t="n">
+        <f aca="false">B77-D77</f>
+        <v>-1476.36</v>
+      </c>
+      <c r="F77" s="4" t="n">
+        <f aca="false">E77/B77</f>
+        <v>-0.0914295764486288</v>
+      </c>
+      <c r="G77" s="4" t="n">
+        <f aca="false">SUM($F$2:F77)</f>
+        <v>-0.779141909952824</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="B78" s="0" t="n">
+        <v>16005.41</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="D78" s="0" t="n">
+        <v>17582.57</v>
+      </c>
+      <c r="E78" s="0" t="n">
+        <f aca="false">B78-D78</f>
+        <v>-1577.16</v>
+      </c>
+      <c r="F78" s="4" t="n">
+        <f aca="false">E78/B78</f>
+        <v>-0.0985391814392759</v>
+      </c>
+      <c r="G78" s="4" t="n">
+        <f aca="false">SUM($F$2:F78)</f>
+        <v>-0.877681091392099</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="5" t="s">
+        <v>213</v>
+      </c>
+      <c r="B79" s="0" t="n">
+        <v>16035.61</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="D79" s="0" t="n">
+        <v>17502.59</v>
+      </c>
+      <c r="E79" s="0" t="n">
+        <f aca="false">B79-D79</f>
+        <v>-1466.98</v>
+      </c>
+      <c r="F79" s="4" t="n">
+        <f aca="false">E79/B79</f>
+        <v>-0.0914826439405797</v>
+      </c>
+      <c r="G79" s="4" t="n">
+        <f aca="false">SUM($F$2:F79)</f>
+        <v>-0.969163735332679</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="5" t="s">
+        <v>214</v>
+      </c>
+      <c r="B80" s="0" t="n">
+        <v>15897.82</v>
+      </c>
+      <c r="C80" s="5" t="s">
+        <v>243</v>
+      </c>
+      <c r="D80" s="0" t="n">
+        <v>17515.73</v>
+      </c>
+      <c r="E80" s="0" t="n">
+        <f aca="false">B80-D80</f>
+        <v>-1617.91</v>
+      </c>
+      <c r="F80" s="4" t="n">
+        <f aca="false">E80/B80</f>
+        <v>-0.101769299186933</v>
+      </c>
+      <c r="G80" s="4" t="n">
+        <f aca="false">SUM($F$2:F80)</f>
+        <v>-1.07093303451961</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="B81" s="0" t="n">
+        <v>15691.62</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="D81" s="0" t="n">
+        <v>17535.39</v>
+      </c>
+      <c r="E81" s="0" t="n">
+        <f aca="false">B81-D81</f>
+        <v>-1843.77</v>
+      </c>
+      <c r="F81" s="4" t="n">
+        <f aca="false">E81/B81</f>
+        <v>-0.117500296336516</v>
+      </c>
+      <c r="G81" s="4" t="n">
+        <f aca="false">SUM($F$2:F81)</f>
+        <v>-1.18843333085613</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="5" t="s">
+        <v>216</v>
+      </c>
+      <c r="B82" s="0" t="n">
+        <v>16012.39</v>
+      </c>
+      <c r="C82" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="D82" s="0" t="n">
+        <v>17633.11</v>
+      </c>
+      <c r="E82" s="0" t="n">
+        <f aca="false">B82-D82</f>
+        <v>-1620.72</v>
+      </c>
+      <c r="F82" s="4" t="n">
+        <f aca="false">E82/B82</f>
+        <v>-0.101216620379594</v>
+      </c>
+      <c r="G82" s="4" t="n">
+        <f aca="false">SUM($F$2:F82)</f>
+        <v>-1.28964995123572</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="5" t="s">
+        <v>217</v>
+      </c>
+      <c r="B83" s="0" t="n">
+        <v>16217.98</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>246</v>
+      </c>
+      <c r="D83" s="0" t="n">
+        <v>17716.66</v>
+      </c>
+      <c r="E83" s="0" t="n">
+        <f aca="false">B83-D83</f>
+        <v>-1498.68</v>
+      </c>
+      <c r="F83" s="4" t="n">
+        <f aca="false">E83/B83</f>
+        <v>-0.0924085490301505</v>
+      </c>
+      <c r="G83" s="4" t="n">
+        <f aca="false">SUM($F$2:F83)</f>
+        <v>-1.38205850026587</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="5" t="s">
+        <v>218</v>
+      </c>
+      <c r="B84" s="0" t="n">
+        <v>16483.76</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="D84" s="0" t="n">
+        <v>17685.09</v>
+      </c>
+      <c r="E84" s="0" t="n">
+        <f aca="false">B84-D84</f>
+        <v>-1201.33</v>
+      </c>
+      <c r="F84" s="4" t="n">
+        <f aca="false">E84/B84</f>
+        <v>-0.0728796099918952</v>
+      </c>
+      <c r="G84" s="4" t="n">
+        <f aca="false">SUM($F$2:F84)</f>
+        <v>-1.45493811025777</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="5" t="s">
+        <v>219</v>
+      </c>
+      <c r="B85" s="0" t="n">
+        <v>16410.96</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="D85" s="0" t="n">
+        <v>17792.75</v>
+      </c>
+      <c r="E85" s="0" t="n">
+        <f aca="false">B85-D85</f>
+        <v>-1381.79</v>
+      </c>
+      <c r="F85" s="4" t="n">
+        <f aca="false">E85/B85</f>
+        <v>-0.0841992180835247</v>
+      </c>
+      <c r="G85" s="4" t="n">
+        <f aca="false">SUM($F$2:F85)</f>
+        <v>-1.53913732834129</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="B86" s="0" t="n">
+        <v>16417.13</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="D86" s="0" t="n">
+        <v>17737</v>
+      </c>
+      <c r="E86" s="0" t="n">
+        <f aca="false">B86-D86</f>
+        <v>-1319.87</v>
+      </c>
+      <c r="F86" s="4" t="n">
+        <f aca="false">E86/B86</f>
+        <v>-0.0803959035470876</v>
+      </c>
+      <c r="G86" s="4" t="n">
+        <f aca="false">SUM($F$2:F86)</f>
+        <v>-1.61953323188838</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="5" t="s">
+        <v>221</v>
+      </c>
+      <c r="B87" s="0" t="n">
+        <v>16610.39</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>250</v>
+      </c>
+      <c r="D87" s="0" t="n">
+        <v>17603.32</v>
+      </c>
+      <c r="E87" s="0" t="n">
+        <f aca="false">B87-D87</f>
+        <v>-992.93</v>
+      </c>
+      <c r="F87" s="4" t="n">
+        <f aca="false">E87/B87</f>
+        <v>-0.0597776451967714</v>
+      </c>
+      <c r="G87" s="4" t="n">
+        <f aca="false">SUM($F$2:F87)</f>
+        <v>-1.67931087708515</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="5" t="s">
+        <v>222</v>
+      </c>
+      <c r="B88" s="0" t="n">
+        <v>16418.84</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>251</v>
+      </c>
+      <c r="D88" s="0" t="n">
+        <v>17716.05</v>
+      </c>
+      <c r="E88" s="0" t="n">
+        <f aca="false">B88-D88</f>
+        <v>-1297.21</v>
+      </c>
+      <c r="F88" s="4" t="n">
+        <f aca="false">E88/B88</f>
+        <v>-0.0790074085623588</v>
+      </c>
+      <c r="G88" s="4" t="n">
+        <f aca="false">SUM($F$2:F88)</f>
+        <v>-1.75831828564751</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="B89" s="0" t="n">
+        <v>16504.38</v>
+      </c>
+      <c r="C89" s="5" t="s">
+        <v>252</v>
+      </c>
+      <c r="D89" s="0" t="n">
+        <v>17541.96</v>
+      </c>
+      <c r="E89" s="0" t="n">
+        <f aca="false">B89-D89</f>
+        <v>-1037.58</v>
+      </c>
+      <c r="F89" s="4" t="n">
+        <f aca="false">E89/B89</f>
+        <v>-0.0628669480465184</v>
+      </c>
+      <c r="G89" s="4" t="n">
+        <f aca="false">SUM($F$2:F89)</f>
+        <v>-1.82118523369403</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B90" s="0" t="n">
+        <v>16712.7</v>
+      </c>
+      <c r="C90" s="5" t="s">
+        <v>253</v>
+      </c>
+      <c r="D90" s="0" t="n">
+        <v>17576.96</v>
+      </c>
+      <c r="E90" s="6" t="n">
+        <f aca="false">D90-B90</f>
+        <v>864.259999999998</v>
+      </c>
+      <c r="F90" s="4" t="n">
+        <f aca="false">E90/B90</f>
+        <v>0.0517127693311074</v>
+      </c>
+      <c r="G90" s="4" t="n">
+        <f aca="false">SUM($F$2:F90)</f>
+        <v>-1.76947246436292</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="5" t="s">
+        <v>225</v>
+      </c>
+      <c r="B91" s="0" t="n">
+        <v>16634.15</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>254</v>
+      </c>
+      <c r="D91" s="0" t="n">
+        <v>17556.41</v>
+      </c>
+      <c r="E91" s="6" t="n">
+        <f aca="false">D91-B91</f>
+        <v>922.259999999998</v>
+      </c>
+      <c r="F91" s="4" t="n">
+        <f aca="false">E91/B91</f>
+        <v>0.0554437707968245</v>
+      </c>
+      <c r="G91" s="4" t="n">
+        <f aca="false">SUM($F$2:F91)</f>
+        <v>-1.7140286935661</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="5" t="s">
+        <v>226</v>
+      </c>
+      <c r="B92" s="0" t="n">
+        <v>16545.67</v>
+      </c>
+      <c r="C92" s="5" t="s">
+        <v>255</v>
+      </c>
+      <c r="D92" s="0" t="n">
+        <v>17721.25</v>
+      </c>
+      <c r="E92" s="6" t="n">
+        <f aca="false">D92-B92</f>
+        <v>1175.58</v>
+      </c>
+      <c r="F92" s="4" t="n">
+        <f aca="false">E92/B92</f>
+        <v>0.0710506132420145</v>
+      </c>
+      <c r="G92" s="4" t="n">
+        <f aca="false">SUM($F$2:F92)</f>
+        <v>-1.64297808032408</v>
       </c>
     </row>
   </sheetData>

</xml_diff>